<commit_message>
Round 2 of identifications
continued
</commit_message>
<xml_diff>
--- a/herbivory/data/herbivoryVideoDataSheet.xlsx
+++ b/herbivory/data/herbivoryVideoDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gleno\OneDrive\Documents\GitHub\photogrammetryNOAA\herbivory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A41FC50-4B80-4A62-8C2B-BA12A25692BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD6216-3D13-40F2-AEA1-4E12F2EB3071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12390" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12390" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="163">
   <si>
     <t>date</t>
   </si>
@@ -496,6 +496,21 @@
   </si>
   <si>
     <t>GP010185</t>
+  </si>
+  <si>
+    <t>IC-C3</t>
+  </si>
+  <si>
+    <t>*almost indistinguishable from yellowtail except for markings on the outside of the caudal fin</t>
+  </si>
+  <si>
+    <t>GH012197</t>
+  </si>
+  <si>
+    <t>GH032197</t>
+  </si>
+  <si>
+    <t>GH042197</t>
   </si>
 </sst>
 </file>
@@ -920,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X210"/>
+  <dimension ref="A1:X213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="J211" sqref="J211"/>
+    <sheetView tabSelected="1" topLeftCell="G196" zoomScale="107" workbookViewId="0">
+      <selection activeCell="K215" sqref="K215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8375,7 +8390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" s="2">
         <v>44119</v>
       </c>
@@ -8410,7 +8425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="2">
         <v>44119</v>
       </c>
@@ -8442,6 +8457,114 @@
         <v>33</v>
       </c>
       <c r="K210" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A211" s="2">
+        <v>44359</v>
+      </c>
+      <c r="B211" t="s">
+        <v>158</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
+      </c>
+      <c r="D211" t="s">
+        <v>160</v>
+      </c>
+      <c r="E211" s="10">
+        <v>0.45277777777777778</v>
+      </c>
+      <c r="F211" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G211" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H211" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I211" s="8">
+        <v>1</v>
+      </c>
+      <c r="J211" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K211" s="8">
+        <v>5</v>
+      </c>
+      <c r="L211" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A212" s="2">
+        <v>44359</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C212" s="8">
+        <v>1</v>
+      </c>
+      <c r="D212" t="s">
+        <v>161</v>
+      </c>
+      <c r="E212" s="10">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="F212" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G212" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H212" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I212" s="8">
+        <v>1</v>
+      </c>
+      <c r="J212" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K212" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A213" s="2">
+        <v>44359</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C213" s="8">
+        <v>1</v>
+      </c>
+      <c r="D213" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E213" s="10">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="F213" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G213" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H213" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I213" s="8">
+        <v>1</v>
+      </c>
+      <c r="J213" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K213" s="8">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Herbivory Data Sheet
I finished C, U, and Z for the July 2022 timepoint. Yay!
</commit_message>
<xml_diff>
--- a/herbivory/data/herbivoryVideoDataSheet.xlsx
+++ b/herbivory/data/herbivoryVideoDataSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookepohlman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookepohlman/Documents/GitHub/photogrammetryNOAA/herbivory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9E4732D-39EF-6643-9037-3E268CF32D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51104E86-36E3-0349-BD91-F341340A1FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="500" windowWidth="27880" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7789" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8257" uniqueCount="507">
   <si>
     <t>date</t>
   </si>
@@ -1471,6 +1471,91 @@
   </si>
   <si>
     <t>GP090253</t>
+  </si>
+  <si>
+    <t>viride</t>
+  </si>
+  <si>
+    <t>Sparisoma viride</t>
+  </si>
+  <si>
+    <t>GP010252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He yanked the whole blade out!
+**Also the camera died and we only got 25 minutes of footage for this assay. This was the only encounter in that time. </t>
+  </si>
+  <si>
+    <t>GH029112</t>
+  </si>
+  <si>
+    <t>GH059112</t>
+  </si>
+  <si>
+    <t>GH069112</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>GH079112</t>
+  </si>
+  <si>
+    <t>GH089112</t>
+  </si>
+  <si>
+    <t>GH023953</t>
+  </si>
+  <si>
+    <t>GH033953</t>
+  </si>
+  <si>
+    <t>GH043953</t>
+  </si>
+  <si>
+    <t>GH063953</t>
+  </si>
+  <si>
+    <t>GH073953</t>
+  </si>
+  <si>
+    <t>GH024332</t>
+  </si>
+  <si>
+    <t>GH034332</t>
+  </si>
+  <si>
+    <t>GH044332</t>
+  </si>
+  <si>
+    <t>GP020069</t>
+  </si>
+  <si>
+    <t>GP030069</t>
+  </si>
+  <si>
+    <t>4,1,2</t>
+  </si>
+  <si>
+    <t>GP040069</t>
+  </si>
+  <si>
+    <t>chrysopterum</t>
+  </si>
+  <si>
+    <t>GH018273</t>
+  </si>
+  <si>
+    <t>GH038273</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>GH048273</t>
+  </si>
+  <si>
+    <t>GH058273</t>
   </si>
 </sst>
 </file>
@@ -1887,11 +1972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1027"/>
+  <dimension ref="A1:Z1082"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="116" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A996" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1031" sqref="I1031"/>
+      <pane ySplit="1" topLeftCell="A1047" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1084" sqref="B1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44978,6 +45063,2264 @@
         <v>2</v>
       </c>
       <c r="N1027" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1028" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1028" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1028" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1028" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="E1028" s="8">
+        <v>0.1277777777777778</v>
+      </c>
+      <c r="F1028" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1028" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1028" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="I1028" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="J1028" s="18">
+        <v>1</v>
+      </c>
+      <c r="K1028" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1028" s="18">
+        <v>5</v>
+      </c>
+      <c r="M1028" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="N1028" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1029" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1029" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1029" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1029" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1029" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="F1029" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1029" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1029" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1029" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1029" s="18">
+        <v>1</v>
+      </c>
+      <c r="K1029" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1029" s="18">
+        <v>2</v>
+      </c>
+      <c r="N1029" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1030" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1030" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1030" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1030" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="E1030" s="8">
+        <v>0.26597222222222222</v>
+      </c>
+      <c r="F1030" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1030" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1030" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1030" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1030" s="18">
+        <v>1</v>
+      </c>
+      <c r="K1030" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1030" s="18">
+        <v>2</v>
+      </c>
+      <c r="N1030" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1031" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1031" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1031" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1031" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="E1031" s="8">
+        <v>0.45902777777777781</v>
+      </c>
+      <c r="F1031" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1031" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1031" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1031" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1031" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1031" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1031" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="N1031" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1032" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1032" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1032" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1032" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E1032" s="8">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="F1032" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1032" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1032" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1032" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1032" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1032" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1032" s="18" t="s">
+        <v>486</v>
+      </c>
+      <c r="N1032" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1033" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1033" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1033" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1033" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E1033" s="8">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="F1033" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1033" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1033" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1033" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1033" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1033" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1033" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="N1033" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1034" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1034" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1034" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1034" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E1034" s="8">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="F1034" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1034" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1034" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1034" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1034" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1034" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1034" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="N1034" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1035" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1035" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1035" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1035" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1035" s="8">
+        <v>0.2076388888888889</v>
+      </c>
+      <c r="F1035" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1035" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1035" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1035" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1035" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1035" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1035" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1035" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1036" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1036" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1036" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1036" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="E1036" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F1036" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1036" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1036" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1036" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1036" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1036" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1036" s="7">
+        <v>5</v>
+      </c>
+      <c r="N1036" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1037" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1037" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1037" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1037" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1037" s="8">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="F1037" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1037" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1037" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1037" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1037" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1037" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1037" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1037" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1038" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1038" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1038" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1038" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1038" s="8">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="F1038" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1038" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1038" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1038" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1038" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1038" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1038" s="12">
+        <v>4</v>
+      </c>
+      <c r="N1038" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1039" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1039" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1039" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1039" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1039" s="8">
+        <v>0.24236111111111111</v>
+      </c>
+      <c r="F1039" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1039" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1039" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1039" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1039" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1039" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1039" s="12">
+        <v>5</v>
+      </c>
+      <c r="N1039" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1040" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1040" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1040" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1040" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1040" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="F1040" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1040" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1040" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1040" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1040" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1040" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1040" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="N1040" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1041" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1041" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1041" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1041" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1041" s="8">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="F1041" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1041" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1041" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1041" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1041" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1041" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1041" s="12">
+        <v>1</v>
+      </c>
+      <c r="N1041" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1042" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1042" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1042" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1042" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1042" s="8">
+        <v>5.8333333333333327E-2</v>
+      </c>
+      <c r="F1042" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1042" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1042" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1042" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1042" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1042" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1042" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1042" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1043" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1043" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1043" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1043" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1043" s="8">
+        <v>0.11319444444444444</v>
+      </c>
+      <c r="F1043" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1043" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1043" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1043" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1043" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1043" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1043" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="N1043" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1044" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1044" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1044" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1044" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1044" s="8">
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="F1044" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1044" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1044" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1044" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1044" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1044" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1044" s="7">
+        <v>2</v>
+      </c>
+      <c r="N1044" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1045" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1045" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1045" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1045" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1045" s="8">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="F1045" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1045" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1045" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1045" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1045" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1045" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1045" s="7">
+        <v>2</v>
+      </c>
+      <c r="N1045" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1046" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1046" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1046" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1046" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="E1046" s="8">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="F1046" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1046" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1046" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1046" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1046" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1046" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1046" s="12">
+        <v>1</v>
+      </c>
+      <c r="N1046" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1047" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1047" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1047" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1047" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1047" s="8">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="F1047" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1047" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1047" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1047" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1047" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1047" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1047" s="12">
+        <v>4</v>
+      </c>
+      <c r="N1047" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1048" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1048" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1048" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1048" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1048" s="8">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="F1048" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1048" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1048" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1048" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1048" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1048" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1048" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="N1048" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1049" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1049" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1049" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1049" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1049" s="8">
+        <v>0.34236111111111112</v>
+      </c>
+      <c r="F1049" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1049" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1049" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1049" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1049" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1049" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1049" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1049" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1050" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1050" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1050" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1050" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1050" s="8">
+        <v>0.34583333333333338</v>
+      </c>
+      <c r="F1050" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1050" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1050" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1050" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1050" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1050" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1050" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="N1050" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1051" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1051" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1051" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1051" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1051" s="8">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="F1051" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1051" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1051" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1051" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1051" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1051" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1051" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1051" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1052" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1052" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1052" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1052" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1052" s="8">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="F1052" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1052" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1052" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1052" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1052" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1052" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1052" s="7">
+        <v>2</v>
+      </c>
+      <c r="N1052" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1053" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1053" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1053" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1053" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1053" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="F1053" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1053" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1053" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1053" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1053" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1053" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1053" s="7">
+        <v>5</v>
+      </c>
+      <c r="N1053" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1054" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1054" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1054" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1054" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1054" s="8">
+        <v>0.40833333333333338</v>
+      </c>
+      <c r="F1054" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1054" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1054" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1054" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1054" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1054" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1054" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1054" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1055" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1055" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1055" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1055" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1055" s="8">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="F1055" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1055" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1055" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1055" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1055" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1055" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1055" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1055" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1056" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1056" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1056" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1056" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="E1056" s="8">
+        <v>0.19166666666666665</v>
+      </c>
+      <c r="F1056" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1056" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1056" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1056" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1056" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1056" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1056" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="N1056" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1057" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1057" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1057" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1057" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="E1057" s="8">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="F1057" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1057" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1057" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1057" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1057" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1057" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1057" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="N1057" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1058" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1058" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1058" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1058" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1058" s="8">
+        <v>0.23055555555555554</v>
+      </c>
+      <c r="F1058" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1058" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1058" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1058" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1058" s="17">
+        <v>1</v>
+      </c>
+      <c r="K1058" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1058" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="N1058" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1059" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1059" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1059" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1059" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1059" s="8">
+        <v>0.4069444444444445</v>
+      </c>
+      <c r="F1059" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1059" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1059" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1059" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1059" s="17">
+        <v>1</v>
+      </c>
+      <c r="K1059" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1059" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="N1059" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1060" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1060" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1060" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1060" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1060" s="8">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="F1060" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1060" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1060" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1060" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1060" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1060" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1060" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1060" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1061" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1061" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1061" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1061" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1061" s="8">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="F1061" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1061" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1061" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1061" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1061" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1061" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1061" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1061" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1062" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1062" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1062" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1062" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1062" s="8">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="F1062" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1062" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1062" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1062" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1062" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1062" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1062" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1062" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1063" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1063" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1063" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1063" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1063" s="8">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="F1063" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1063" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1063" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1063" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1063" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1063" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1063" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="N1063" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1064" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1064" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1064" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1064" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1064" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F1064" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1064" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1064" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1064" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1064" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1064" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1064" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1064" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1065" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1065" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1065" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1065" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1065" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F1065" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1065" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1065" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1065" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1065" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1065" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1065" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="N1065" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1066" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1066" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1066" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1066" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1066" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F1066" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1066" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1066" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1066" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1066" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1066" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1066" s="7">
+        <v>4</v>
+      </c>
+      <c r="N1066" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1067" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1067" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1067" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1067" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1067" s="8">
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="F1067" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1067" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1067" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1067" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1067" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1067" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1067" s="7">
+        <v>4</v>
+      </c>
+      <c r="N1067" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1068" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1068" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1068" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1068" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1068" s="8">
+        <v>0.13125000000000001</v>
+      </c>
+      <c r="F1068" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1068" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1068" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1068" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1068" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1068" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1068" s="7">
+        <v>5</v>
+      </c>
+      <c r="N1068" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1069" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1069" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1069" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1069" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1069" s="8">
+        <v>0.16944444444444443</v>
+      </c>
+      <c r="F1069" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1069" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1069" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1069" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1069" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1069" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1069" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="N1069" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1070" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1070" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1070" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1070" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1070" s="8">
+        <v>0.21458333333333335</v>
+      </c>
+      <c r="F1070" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1070" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1070" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1070" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1070" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1070" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1070" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="N1070" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1071" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1071" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1071" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1071" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1071" s="8">
+        <v>0.29305555555555557</v>
+      </c>
+      <c r="F1071" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1071" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1071" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1071" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1071" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1071" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1071" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="N1071" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1072" s="6">
+        <v>44761</v>
+      </c>
+      <c r="B1072" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1072" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1072" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1072" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="F1072" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1072" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1072" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1072" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1072" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1072" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1072" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1072" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1073" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1073" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1073" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1073" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="E1073" s="8">
+        <v>0.21388888888888891</v>
+      </c>
+      <c r="F1073" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1073" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1073" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1073" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1073" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1073" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1073" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="N1073" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1074" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1074" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1074" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1074" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="E1074" s="8">
+        <v>0.24097222222222223</v>
+      </c>
+      <c r="F1074" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1074" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1074" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1074" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1074" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1074" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1074" s="7">
+        <v>3</v>
+      </c>
+      <c r="N1074" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1075" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1075" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1075" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1075" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1075" s="8">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="F1075" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1075" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1075" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1075" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1075" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1075" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1075" s="7">
+        <v>2</v>
+      </c>
+      <c r="N1075" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1076" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1076" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1076" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1076" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1076" s="8">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="F1076" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1076" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1076" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1076" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1076" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1076" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1076" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="N1076" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1077" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1077" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1077" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1077" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1077" s="8">
+        <v>0.3444444444444445</v>
+      </c>
+      <c r="F1077" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1077" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1077" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1077" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1077" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1077" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1077" s="12">
+        <v>5</v>
+      </c>
+      <c r="N1077" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1078" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1078" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1078" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1078" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1078" s="8">
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="F1078" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1078" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1078" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1078" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="J1078" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1078" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1078" s="12">
+        <v>5</v>
+      </c>
+      <c r="N1078" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1079" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1079" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1079" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1079" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1079" s="8">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="F1079" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1079" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1079" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1079" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1079" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1079" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1079" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1079" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1080" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1080" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1080" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1080" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1080" s="8">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="F1080" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1080" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1080" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1080" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1080" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1080" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1080" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="N1080" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1081" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1081" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1081" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1081" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1081" s="8">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F1081" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1081" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1081" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1081" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1081" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1081" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1081" s="7">
+        <v>4</v>
+      </c>
+      <c r="N1081" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1082" s="6">
+        <v>44752</v>
+      </c>
+      <c r="B1082" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1082" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1082" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="E1082" s="8">
+        <v>0.1173611111111111</v>
+      </c>
+      <c r="F1082" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1082" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1082" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1082" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1082" s="16">
+        <v>1</v>
+      </c>
+      <c r="K1082" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1082" s="12">
+        <v>3</v>
+      </c>
+      <c r="N1082" s="9" t="s">
         <v>384</v>
       </c>
     </row>

</xml_diff>